<commit_message>
Precision, recall y g-means del baseline (Issue #88)
En este commit actualizo el documento "Baselines retinologos" para incluir el cálculo de las métricas: precision, recall y g-means en el baseline de los retinólogos. Las funciones que he empleado salen del paquete metrics de scikit learn. Los resultados obtenidos les he añadido en la tabla de resultados finales, para compararlos con la tabla de valores que estoy sacando de Scayle.
</commit_message>
<xml_diff>
--- a/Resultados/CV DA completo/Resultados EMD CV DA.xlsx
+++ b/Resultados/CV DA completo/Resultados EMD CV DA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\TFG\Transfer-Learning-EDM\Resultados\CV DA completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E006F4-8870-44AD-80DA-00E91AB8B370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94BD7DDA-6359-4D63-B88A-840B903AADA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -2015,8 +2015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AU884"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M336" zoomScale="81" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="AF345" sqref="AF345"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU11" sqref="AU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2045,6 +2045,10 @@
     <col min="37" max="37" width="12.77734375" customWidth="1"/>
     <col min="38" max="38" width="20.6640625" customWidth="1"/>
     <col min="41" max="41" width="17.33203125" customWidth="1"/>
+    <col min="44" max="44" width="12.33203125" customWidth="1"/>
+    <col min="45" max="45" width="13.33203125" customWidth="1"/>
+    <col min="46" max="46" width="12.5546875" customWidth="1"/>
+    <col min="47" max="47" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.3">
@@ -2310,9 +2314,15 @@
       <c r="AR3" s="16">
         <v>0.78</v>
       </c>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15"/>
+      <c r="AS3" s="16">
+        <v>0.73170000000000002</v>
+      </c>
+      <c r="AT3" s="16">
+        <v>0.83</v>
+      </c>
+      <c r="AU3" s="16">
+        <v>0.82</v>
+      </c>
     </row>
     <row r="4" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -2446,9 +2456,15 @@
       <c r="AR4" s="18">
         <v>0.83</v>
       </c>
-      <c r="AS4" s="17"/>
-      <c r="AT4" s="17"/>
-      <c r="AU4" s="17"/>
+      <c r="AS4" s="18">
+        <v>0.60409999999999997</v>
+      </c>
+      <c r="AT4" s="18">
+        <v>0.87</v>
+      </c>
+      <c r="AU4" s="18">
+        <v>0.76</v>
+      </c>
     </row>
     <row r="5" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
@@ -19936,7 +19952,7 @@
         <v>3</v>
       </c>
       <c r="AC151" s="3">
-        <f t="shared" ref="AC151:AL151" si="279">(J735+J737+J739+J741+J743)</f>
+        <f t="shared" ref="AC151:AE151" si="279">(J735+J737+J739+J741+J743)</f>
         <v>25</v>
       </c>
       <c r="AD151" s="3">
@@ -19952,7 +19968,7 @@
         <v>0.63913043478260856</v>
       </c>
       <c r="AG151" s="3">
-        <f t="shared" ref="AG151:AL151" si="280">(N735+N737+N739+N741+N743)/5</f>
+        <f t="shared" ref="AG151:AK151" si="280">(N735+N737+N739+N741+N743)/5</f>
         <v>0.59836547891467762</v>
       </c>
       <c r="AH151" s="3">
@@ -20057,7 +20073,7 @@
         <v>14</v>
       </c>
       <c r="AC152" s="3">
-        <f t="shared" ref="AC152:AL152" si="281">(J736+J738+J740+J742+J744)</f>
+        <f t="shared" ref="AC152:AE152" si="281">(J736+J738+J740+J742+J744)</f>
         <v>30</v>
       </c>
       <c r="AD152" s="3">
@@ -20073,7 +20089,7 @@
         <v>0.53766233766233706</v>
       </c>
       <c r="AG152" s="3">
-        <f t="shared" ref="AG152:AL152" si="282">(N736+N738+N740+N742+N744)/5</f>
+        <f t="shared" ref="AG152:AK152" si="282">(N736+N738+N740+N742+N744)/5</f>
         <v>0.51206094559035686</v>
       </c>
       <c r="AH152" s="3">
@@ -20904,7 +20920,7 @@
         <v>10</v>
       </c>
       <c r="AC159" s="3">
-        <f t="shared" ref="AC159:AL159" si="295">(J775+J777+J779+J781+J783)</f>
+        <f t="shared" ref="AC159:AE159" si="295">(J775+J777+J779+J781+J783)</f>
         <v>18</v>
       </c>
       <c r="AD159" s="3">
@@ -20920,7 +20936,7 @@
         <v>0.74999999999999956</v>
       </c>
       <c r="AG159" s="3">
-        <f t="shared" ref="AG159:AL159" si="296">(N775+N777+N779+N781+N783)/5</f>
+        <f t="shared" ref="AG159:AK159" si="296">(N775+N777+N779+N781+N783)/5</f>
         <v>0.73811603571194317</v>
       </c>
       <c r="AH159" s="3">
@@ -21025,7 +21041,7 @@
         <v>22</v>
       </c>
       <c r="AC160" s="3">
-        <f t="shared" ref="AC160:AL160" si="297">(J776+J778+J780+J782+J784)</f>
+        <f t="shared" ref="AC160:AE160" si="297">(J776+J778+J780+J782+J784)</f>
         <v>22</v>
       </c>
       <c r="AD160" s="3">
@@ -21041,7 +21057,7 @@
         <v>0.56666666666666632</v>
       </c>
       <c r="AG160" s="3">
-        <f t="shared" ref="AG160:AL160" si="298">(N776+N778+N780+N782+N784)/5</f>
+        <f t="shared" ref="AG160:AK160" si="298">(N776+N778+N780+N782+N784)/5</f>
         <v>0.57780219780219744</v>
       </c>
       <c r="AH160" s="3">
@@ -21146,7 +21162,7 @@
         <v>10</v>
       </c>
       <c r="AC161" s="3">
-        <f t="shared" ref="AC161:AL161" si="299">J785+J787+J789+J791+J793</f>
+        <f t="shared" ref="AC161:AE161" si="299">J785+J787+J789+J791+J793</f>
         <v>18</v>
       </c>
       <c r="AD161" s="3">
@@ -21162,7 +21178,7 @@
         <v>0.73391304347826036</v>
       </c>
       <c r="AG161" s="3">
-        <f t="shared" ref="AG161:AL161" si="300">(N785+N787+N789+N791+N793)/5</f>
+        <f t="shared" ref="AG161:AK161" si="300">(N785+N787+N789+N791+N793)/5</f>
         <v>0.72279503105590026</v>
       </c>
       <c r="AH161" s="3">
@@ -21267,7 +21283,7 @@
         <v>22</v>
       </c>
       <c r="AC162" s="3">
-        <f t="shared" ref="AC162:AL162" si="301">J786+J788+J790+J792+J794</f>
+        <f t="shared" ref="AC162:AE162" si="301">J786+J788+J790+J792+J794</f>
         <v>22</v>
       </c>
       <c r="AD162" s="3">
@@ -21283,7 +21299,7 @@
         <v>0.54761904761904734</v>
       </c>
       <c r="AG162" s="3">
-        <f t="shared" ref="AG162:AL162" si="302">(N786+N788+N790+N792+N794)/5</f>
+        <f t="shared" ref="AG162:AK162" si="302">(N786+N788+N790+N792+N794)/5</f>
         <v>0.55416583416583376</v>
       </c>
       <c r="AH162" s="3">
@@ -21388,7 +21404,7 @@
         <v>7</v>
       </c>
       <c r="AC163" s="3">
-        <f t="shared" ref="AC163:AL164" si="303">(J795+J797+J799+J801+J803)</f>
+        <f t="shared" ref="AC163:AE164" si="303">(J795+J797+J799+J801+J803)</f>
         <v>26</v>
       </c>
       <c r="AD163" s="3">
@@ -21404,7 +21420,7 @@
         <v>0.65175983436852958</v>
       </c>
       <c r="AG163" s="3">
-        <f t="shared" ref="AG163:AL163" si="304">(N795+N797+N799+N801+N803)/5</f>
+        <f t="shared" ref="AG163:AK163" si="304">(N795+N797+N799+N801+N803)/5</f>
         <v>0.57799019191268675</v>
       </c>
       <c r="AH163" s="3">
@@ -21505,7 +21521,7 @@
         <v>39</v>
       </c>
       <c r="AB164" s="3">
-        <f t="shared" ref="AB164:AB165" si="305">(I796+I798+I800+I802+I804)</f>
+        <f t="shared" ref="AB164" si="305">(I796+I798+I800+I802+I804)</f>
         <v>19</v>
       </c>
       <c r="AC164" s="3">
@@ -21525,7 +21541,7 @@
         <v>0.65683982683982656</v>
       </c>
       <c r="AG164" s="3">
-        <f t="shared" ref="AG164:AL164" si="306">(N796+N798+N800+N802+N804)/5</f>
+        <f t="shared" ref="AG164:AK164" si="306">(N796+N798+N800+N802+N804)/5</f>
         <v>0.659805387719826</v>
       </c>
       <c r="AH164" s="3">
@@ -21630,7 +21646,7 @@
         <v>2</v>
       </c>
       <c r="AC165" s="3">
-        <f t="shared" ref="AC165:AL165" si="307">(J805+J807+J809+J811+J813)</f>
+        <f t="shared" ref="AC165:AE165" si="307">(J805+J807+J809+J811+J813)</f>
         <v>26</v>
       </c>
       <c r="AD165" s="3">
@@ -21646,7 +21662,7 @@
         <v>0.6917391304347823</v>
       </c>
       <c r="AG165" s="3">
-        <f t="shared" ref="AG165:AL165" si="308">(N805+N807+N809+N811+N813)/5</f>
+        <f t="shared" ref="AG165:AK165" si="308">(N805+N807+N809+N811+N813)/5</f>
         <v>0.60803122258300801</v>
       </c>
       <c r="AH165" s="3">
@@ -21751,7 +21767,7 @@
         <v>13</v>
       </c>
       <c r="AC166" s="3">
-        <f t="shared" ref="AC166:AL166" si="309">(J806+J808+J810+J812+J814)</f>
+        <f t="shared" ref="AC166:AE166" si="309">(J806+J808+J810+J812+J814)</f>
         <v>31</v>
       </c>
       <c r="AD166" s="3">
@@ -21767,7 +21783,7 @@
         <v>0.63160173160173072</v>
       </c>
       <c r="AG166" s="3">
-        <f t="shared" ref="AG166:AL166" si="310">(N806+N808+N810+N812+N814)/5</f>
+        <f t="shared" ref="AG166:AK166" si="310">(N806+N808+N810+N812+N814)/5</f>
         <v>0.60884644766997686</v>
       </c>
       <c r="AH166" s="3">
@@ -21872,7 +21888,7 @@
         <v>5</v>
       </c>
       <c r="AC167" s="3">
-        <f t="shared" ref="AC167:AL167" si="311">(J815+J817+J819+J821+J823)</f>
+        <f t="shared" ref="AC167:AE167" si="311">(J815+J817+J819+J821+J823)</f>
         <v>23</v>
       </c>
       <c r="AD167" s="3">
@@ -21888,7 +21904,7 @@
         <v>0.62826086956521698</v>
       </c>
       <c r="AG167" s="3">
-        <f t="shared" ref="AG167:AL167" si="312">(N815+N817+N819+N821+N823)/5</f>
+        <f t="shared" ref="AG167:AK167" si="312">(N815+N817+N819+N821+N823)/5</f>
         <v>0.59200246994297312</v>
       </c>
       <c r="AH167" s="3">
@@ -21993,7 +22009,7 @@
         <v>17</v>
       </c>
       <c r="AC168" s="3">
-        <f t="shared" ref="AC168:AL168" si="313">(J816+J818+J820+J822+J824)</f>
+        <f t="shared" ref="AC168:AE168" si="313">(J816+J818+J820+J822+J824)</f>
         <v>27</v>
       </c>
       <c r="AD168" s="3">
@@ -22009,7 +22025,7 @@
         <v>0.59307359307359275</v>
       </c>
       <c r="AG168" s="3">
-        <f t="shared" ref="AG168:AL168" si="314">(N816+N818+N820+N822+N824)/5</f>
+        <f t="shared" ref="AG168:AK168" si="314">(N816+N818+N820+N822+N824)/5</f>
         <v>0.59203669346526455</v>
       </c>
       <c r="AH168" s="3">
@@ -22114,7 +22130,7 @@
         <v>3</v>
       </c>
       <c r="AC169" s="3">
-        <f t="shared" ref="AC169:AL169" si="315">(J825+J827+J829+J831+J833)</f>
+        <f t="shared" ref="AC169:AE169" si="315">(J825+J827+J829+J831+J833)</f>
         <v>25</v>
       </c>
       <c r="AD169" s="3">
@@ -22130,7 +22146,7 @@
         <v>0.70260869565217343</v>
       </c>
       <c r="AG169" s="3">
-        <f t="shared" ref="AG169:AL169" si="316">(N825+N827+N829+N831+N833)/5</f>
+        <f t="shared" ref="AG169:AK169" si="316">(N825+N827+N829+N831+N833)/5</f>
         <v>0.61828075946870065</v>
       </c>
       <c r="AH169" s="3">
@@ -22235,7 +22251,7 @@
         <v>15</v>
       </c>
       <c r="AC170" s="3">
-        <f t="shared" ref="AC170:AL170" si="317">(J826+J828+J830+J832+J834)</f>
+        <f t="shared" ref="AC170:AE170" si="317">(J826+J828+J830+J832+J834)</f>
         <v>29</v>
       </c>
       <c r="AD170" s="3">
@@ -22251,7 +22267,7 @@
         <v>0.61255411255411185</v>
       </c>
       <c r="AG170" s="3">
-        <f t="shared" ref="AG170:AL170" si="318">(N826+N828+N830+N832+N834)/5</f>
+        <f t="shared" ref="AG170:AK170" si="318">(N826+N828+N830+N832+N834)/5</f>
         <v>0.59640669490936815</v>
       </c>
       <c r="AH170" s="3">
@@ -22356,7 +22372,7 @@
         <v>6</v>
       </c>
       <c r="AC171" s="3">
-        <f t="shared" ref="AC171:AL171" si="319">(J835+J837+J839+J841+J843)</f>
+        <f t="shared" ref="AC171:AE171" si="319">(J835+J837+J839+J841+J843)</f>
         <v>22</v>
       </c>
       <c r="AD171" s="3">
@@ -22372,7 +22388,7 @@
         <v>0.73391304347826036</v>
       </c>
       <c r="AG171" s="3">
-        <f t="shared" ref="AG171:AL171" si="320">(N835+N837+N839+N841+N843)/5</f>
+        <f t="shared" ref="AG171:AK171" si="320">(N835+N837+N839+N841+N843)/5</f>
         <v>0.67208539622528241</v>
       </c>
       <c r="AH171" s="3">
@@ -22477,7 +22493,7 @@
         <v>11</v>
       </c>
       <c r="AC172" s="3">
-        <f t="shared" ref="AC172:AL172" si="321">(J836+J838+J840+J842+J844)</f>
+        <f t="shared" ref="AC172:AE172" si="321">(J836+J838+J840+J842+J844)</f>
         <v>33</v>
       </c>
       <c r="AD172" s="3">
@@ -22493,7 +22509,7 @@
         <v>0.54545454545454475</v>
       </c>
       <c r="AG172" s="3">
-        <f t="shared" ref="AG172:AL172" si="322">(N836+N838+N840+N842+N844)/5</f>
+        <f t="shared" ref="AG172:AK172" si="322">(N836+N838+N840+N842+N844)/5</f>
         <v>0.47942279942279897</v>
       </c>
       <c r="AH172" s="3">
@@ -22598,7 +22614,7 @@
         <v>2</v>
       </c>
       <c r="AC173" s="3">
-        <f t="shared" ref="AC173:AL173" si="323">(J845+J847+J849+J851+J853)</f>
+        <f t="shared" ref="AC173:AE173" si="323">(J845+J847+J849+J851+J853)</f>
         <v>26</v>
       </c>
       <c r="AD173" s="3">
@@ -22614,7 +22630,7 @@
         <v>0.62695652173913019</v>
       </c>
       <c r="AG173" s="3">
-        <f t="shared" ref="AG173:AL173" si="324">(N845+N847+N849+N851+N853)/5</f>
+        <f t="shared" ref="AG173:AK173" si="324">(N845+N847+N849+N851+N853)/5</f>
         <v>0.57006864988558337</v>
       </c>
       <c r="AH173" s="3">
@@ -22719,7 +22735,7 @@
         <v>10</v>
       </c>
       <c r="AC174" s="3">
-        <f t="shared" ref="AC174:AL174" si="325">(J846+J848+J850+J852+J854)</f>
+        <f t="shared" ref="AC174:AE174" si="325">(J846+J848+J850+J852+J854)</f>
         <v>34</v>
       </c>
       <c r="AD174" s="3">
@@ -22735,7 +22751,7 @@
         <v>0.53852813852813819</v>
       </c>
       <c r="AG174" s="3">
-        <f t="shared" ref="AG174:AL174" si="326">(N846+N848+N850+N852+N854)/5</f>
+        <f t="shared" ref="AG174:AK174" si="326">(N846+N848+N850+N852+N854)/5</f>
         <v>0.52248803827751167</v>
       </c>
       <c r="AH174" s="3">
@@ -22840,7 +22856,7 @@
         <v>2</v>
       </c>
       <c r="AC175" s="3">
-        <f t="shared" ref="AC175:AL175" si="327">(J855+J857+J859+J861+J863)</f>
+        <f t="shared" ref="AC175:AE175" si="327">(J855+J857+J859+J861+J863)</f>
         <v>26</v>
       </c>
       <c r="AD175" s="3">
@@ -22856,7 +22872,7 @@
         <v>0.55826086956521725</v>
       </c>
       <c r="AG175" s="3">
-        <f t="shared" ref="AG175:AL175" si="328">(N855+N857+N859+N861+N863)/5</f>
+        <f t="shared" ref="AG175:AK175" si="328">(N855+N857+N859+N861+N863)/5</f>
         <v>0.54201690821256021</v>
       </c>
       <c r="AH175" s="3">
@@ -22961,7 +22977,7 @@
         <v>14</v>
       </c>
       <c r="AC176" s="3">
-        <f t="shared" ref="AC176:AL176" si="329">(J856+J858+J860+J862+J864)</f>
+        <f t="shared" ref="AC176:AE176" si="329">(J856+J858+J860+J862+J864)</f>
         <v>30</v>
       </c>
       <c r="AD176" s="3">
@@ -22977,7 +22993,7 @@
         <v>0.59393939393939343</v>
       </c>
       <c r="AG176" s="3">
-        <f t="shared" ref="AG176:AL176" si="330">(N856+N858+N860+N862+N864)/5</f>
+        <f t="shared" ref="AG176:AK176" si="330">(N856+N858+N860+N862+N864)/5</f>
         <v>0.60016496661233454</v>
       </c>
       <c r="AH176" s="3">
@@ -23082,7 +23098,7 @@
         <v>6</v>
       </c>
       <c r="AC177" s="3">
-        <f t="shared" ref="AC177:AL177" si="331">(J865+J867+J869+J871+J873)</f>
+        <f t="shared" ref="AC177:AE177" si="331">(J865+J867+J869+J871+J873)</f>
         <v>22</v>
       </c>
       <c r="AD177" s="3">
@@ -23098,7 +23114,7 @@
         <v>0.72391304347826035</v>
       </c>
       <c r="AG177" s="3">
-        <f t="shared" ref="AG177:AL177" si="332">(N865+N867+N869+N871+N873)/5</f>
+        <f t="shared" ref="AG177:AK177" si="332">(N865+N867+N869+N871+N873)/5</f>
         <v>0.65255577507094742</v>
       </c>
       <c r="AH177" s="3">
@@ -23203,7 +23219,7 @@
         <v>20</v>
       </c>
       <c r="AC178" s="3">
-        <f t="shared" ref="AC178:AL178" si="333">(J866+J868+J870+J872+J874)</f>
+        <f t="shared" ref="AC178:AE178" si="333">(J866+J868+J870+J872+J874)</f>
         <v>24</v>
       </c>
       <c r="AD178" s="3">
@@ -23219,7 +23235,7 @@
         <v>0.56623376623376576</v>
       </c>
       <c r="AG178" s="3">
-        <f t="shared" ref="AG178:AL178" si="334">(N866+N868+N870+N872+N874)/5</f>
+        <f t="shared" ref="AG178:AK178" si="334">(N866+N868+N870+N872+N874)/5</f>
         <v>0.56306748806748752</v>
       </c>
       <c r="AH178" s="3">
@@ -23324,7 +23340,7 @@
         <v>7</v>
       </c>
       <c r="AC179" s="3">
-        <f t="shared" ref="AC179:AL179" si="335">(J875+J877+J879+J881+J883)</f>
+        <f t="shared" ref="AC179:AE179" si="335">(J875+J877+J879+J881+J883)</f>
         <v>21</v>
       </c>
       <c r="AD179" s="3">
@@ -23340,7 +23356,7 @@
         <v>0.71260869565217333</v>
       </c>
       <c r="AG179" s="3">
-        <f t="shared" ref="AG179:AL179" si="336">(N875+N877+N879+N881+N883)/5</f>
+        <f t="shared" ref="AG179:AK179" si="336">(N875+N877+N879+N881+N883)/5</f>
         <v>0.67781962639887183</v>
       </c>
       <c r="AH179" s="3">
@@ -23445,7 +23461,7 @@
         <v>17</v>
       </c>
       <c r="AC180" s="3">
-        <f t="shared" ref="AC180:AL180" si="337">(J876+J878+J880+J882+J884)</f>
+        <f t="shared" ref="AC180:AE180" si="337">(J876+J878+J880+J882+J884)</f>
         <v>27</v>
       </c>
       <c r="AD180" s="3">
@@ -23461,7 +23477,7 @@
         <v>0.58441558441558372</v>
       </c>
       <c r="AG180" s="3">
-        <f t="shared" ref="AG180:AL180" si="338">(N876+N878+N880+N882+N884)/5</f>
+        <f t="shared" ref="AG180:AK180" si="338">(N876+N878+N880+N882+N884)/5</f>
         <v>0.56277415395062425</v>
       </c>
       <c r="AH180" s="3">

</xml_diff>